<commit_message>
added support for models trained  on colab, train-info updated
</commit_message>
<xml_diff>
--- a/TRAIN-INFO.xlsx
+++ b/TRAIN-INFO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>POS Tagging</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>a100</t>
-  </si>
-  <si>
-    <t>rtx5071</t>
   </si>
 </sst>
 </file>
@@ -426,9 +423,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O28" sqref="O28"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +536,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -559,8 +556,26 @@
       <c r="G3" t="s">
         <v>5</v>
       </c>
+      <c r="H3">
+        <v>0.73050000000000004</v>
+      </c>
+      <c r="I3">
+        <v>0.65649999999999997</v>
+      </c>
+      <c r="J3">
+        <v>0.73440000000000005</v>
+      </c>
+      <c r="K3">
+        <v>0.76970000000000005</v>
+      </c>
+      <c r="L3">
+        <v>0.70220000000000005</v>
+      </c>
+      <c r="M3">
+        <v>0.67</v>
+      </c>
       <c r="N3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -609,7 +624,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -628,6 +643,24 @@
       </c>
       <c r="G5" t="s">
         <v>5</v>
+      </c>
+      <c r="H5">
+        <v>0.84230000000000005</v>
+      </c>
+      <c r="I5">
+        <v>0.81910000000000005</v>
+      </c>
+      <c r="J5">
+        <v>0.84419999999999995</v>
+      </c>
+      <c r="K5">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="L5">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="M5">
+        <v>0.82220000000000004</v>
       </c>
       <c r="N5" t="s">
         <v>19</v>

</xml_diff>